<commit_message>
Trained the ML model with some more datasets
</commit_message>
<xml_diff>
--- a/static/ModelTrainingCode/TaskPriorityData.xlsx
+++ b/static/ModelTrainingCode/TaskPriorityData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="169">
   <si>
     <t>Finish the quarterly report before the deadline</t>
   </si>
@@ -227,6 +227,300 @@
   </si>
   <si>
     <t>Task Priority</t>
+  </si>
+  <si>
+    <t>Submit the progress report to the project manager</t>
+  </si>
+  <si>
+    <t>Follow up with the vendor for product delivery</t>
+  </si>
+  <si>
+    <t>Coordinate with the development team for bug fixing</t>
+  </si>
+  <si>
+    <t>Prepare the training materials for new hires</t>
+  </si>
+  <si>
+    <t>Review and update the marketing campaign strategy</t>
+  </si>
+  <si>
+    <t>Approve the budget allocation for the upcoming project</t>
+  </si>
+  <si>
+    <t>Update the company website with new product information</t>
+  </si>
+  <si>
+    <t>Conduct market research for new product launch</t>
+  </si>
+  <si>
+    <t>Coordinate with the IT department for system upgrades</t>
+  </si>
+  <si>
+    <t>Analyze financial reports and prepare quarterly statements</t>
+  </si>
+  <si>
+    <t>Attend the industry conference to network with potential clients</t>
+  </si>
+  <si>
+    <t>Develop a training program for employee skill enhancement</t>
+  </si>
+  <si>
+    <t>Review and optimize website performance for better user experience</t>
+  </si>
+  <si>
+    <t>Manage inventory levels and reorder stock when necessary</t>
+  </si>
+  <si>
+    <t>Collaborate with the design team on creating new product prototypes</t>
+  </si>
+  <si>
+    <t>Create and deliver sales presentations to prospective customers</t>
+  </si>
+  <si>
+    <t>Conduct performance appraisals for team members</t>
+  </si>
+  <si>
+    <t>Implement new software systems to improve workflow efficiency</t>
+  </si>
+  <si>
+    <t>Lead strategic planning sessions to set company goals</t>
+  </si>
+  <si>
+    <t>Coordinate with external auditors for financial statement reviews</t>
+  </si>
+  <si>
+    <t>Develop marketing materials for product launch campaigns</t>
+  </si>
+  <si>
+    <t>Respond to customer inquiries and provide prompt assistance</t>
+  </si>
+  <si>
+    <t>Monitor project progress and update stakeholders on status</t>
+  </si>
+  <si>
+    <t>Coordinate with suppliers for timely delivery of materials</t>
+  </si>
+  <si>
+    <t>Analyze customer feedback and recommend product improvements</t>
+  </si>
+  <si>
+    <t>Lead cross-functional teams in implementing process improvements</t>
+  </si>
+  <si>
+    <t>Prepare and present financial reports to executive management</t>
+  </si>
+  <si>
+    <t>Resolve customer complaints and ensure customer satisfaction</t>
+  </si>
+  <si>
+    <t>Monitor market trends and competitors' activities</t>
+  </si>
+  <si>
+    <t>Manage social media accounts and engage with followers</t>
+  </si>
+  <si>
+    <t>Develop and implement employee training programs</t>
+  </si>
+  <si>
+    <t>Research and propose cost-saving initiatives</t>
+  </si>
+  <si>
+    <t>Review and finalize the project timeline</t>
+  </si>
+  <si>
+    <t>Coordinate with the marketing team for campaign execution</t>
+  </si>
+  <si>
+    <t>Prepare the monthly sales report for management review</t>
+  </si>
+  <si>
+    <t>Update the customer database with new contact information</t>
+  </si>
+  <si>
+    <t>Respond to urgent customer inquiries via phone and email</t>
+  </si>
+  <si>
+    <t>Conduct product training sessions for the sales team</t>
+  </si>
+  <si>
+    <t>Analyze market data and identify new business opportunities</t>
+  </si>
+  <si>
+    <t>Develop and implement customer retention strategies</t>
+  </si>
+  <si>
+    <t>Coordinate with the HR department for recruitment activities</t>
+  </si>
+  <si>
+    <t>Prepare and present project proposals to potential clients</t>
+  </si>
+  <si>
+    <t>Follow up with suppliers for price negotiations and order placement</t>
+  </si>
+  <si>
+    <t>Review and approve expense reports for reimbursement</t>
+  </si>
+  <si>
+    <t>Monitor and analyze website traffic and performance metrics</t>
+  </si>
+  <si>
+    <t>Attend industry conferences to stay updated on market trends</t>
+  </si>
+  <si>
+    <t>Prepare and conduct team-building activities for staff members</t>
+  </si>
+  <si>
+    <t>Coordinate with the finance department for budget planning</t>
+  </si>
+  <si>
+    <t>Review and update company policies and procedures</t>
+  </si>
+  <si>
+    <t>Respond to high-priority customer support tickets</t>
+  </si>
+  <si>
+    <t>Conduct quality control checks on finished products</t>
+  </si>
+  <si>
+    <t>Develop sales strategies to achieve revenue targets</t>
+  </si>
+  <si>
+    <t>Coordinate with the logistics team for product shipments</t>
+  </si>
+  <si>
+    <t>Review and analyze customer feedback surveys</t>
+  </si>
+  <si>
+    <t>Prepare and deliver training sessions for new employees</t>
+  </si>
+  <si>
+    <t>Monitor project expenses and ensure budget adherence</t>
+  </si>
+  <si>
+    <t>Respond to urgent email inquiries from clients</t>
+  </si>
+  <si>
+    <t>Conduct market research to identify target demographics</t>
+  </si>
+  <si>
+    <t>Collaborate with the design team to create new product packaging</t>
+  </si>
+  <si>
+    <t>Review and approve content for marketing materials</t>
+  </si>
+  <si>
+    <t>Prepare sales forecasts for upcoming quarters</t>
+  </si>
+  <si>
+    <t>Coordinate with the IT department for system maintenance</t>
+  </si>
+  <si>
+    <t>Analyze sales data and identify trends for strategic planning</t>
+  </si>
+  <si>
+    <t>Attend product training sessions to stay updated on features</t>
+  </si>
+  <si>
+    <t>Prepare and present financial reports to stakeholders</t>
+  </si>
+  <si>
+    <t>Respond to customer complaints and resolve issues</t>
+  </si>
+  <si>
+    <t>Conduct competitor analysis to inform marketing strategies</t>
+  </si>
+  <si>
+    <t>Develop and implement employee recognition programs</t>
+  </si>
+  <si>
+    <t>Coordinate with the legal department for contract reviews</t>
+  </si>
+  <si>
+    <t>Review and approve time-off requests for employees</t>
+  </si>
+  <si>
+    <t>Create and deliver presentations at industry conferences</t>
+  </si>
+  <si>
+    <t>Analyze inventory levels and optimize stock management</t>
+  </si>
+  <si>
+    <t>Follow up with leads generated from marketing campaigns</t>
+  </si>
+  <si>
+    <t>Coordinate with the engineering team for product development</t>
+  </si>
+  <si>
+    <t>Review and update the company's social media strategy</t>
+  </si>
+  <si>
+    <t>Prepare and deliver performance evaluations for team members</t>
+  </si>
+  <si>
+    <t>Analyze customer buying patterns and recommend product improvements</t>
+  </si>
+  <si>
+    <t>Coordinate with the operations team for process improvements</t>
+  </si>
+  <si>
+    <t>Prepare and present project progress reports to stakeholders</t>
+  </si>
+  <si>
+    <t>Respond to customer inquiries on social media platforms</t>
+  </si>
+  <si>
+    <t>Conduct market segmentation analysis for targeted marketing</t>
+  </si>
+  <si>
+    <t>Develop and implement safety protocols in the workplace</t>
+  </si>
+  <si>
+    <t>Coordinate with suppliers to ensure timely delivery of materials</t>
+  </si>
+  <si>
+    <t>Review and update employee benefits and compensation plans</t>
+  </si>
+  <si>
+    <t>Coordinate with the research and development team for new product ideas</t>
+  </si>
+  <si>
+    <t>Analyze customer satisfaction surveys and identify areas for improvement</t>
+  </si>
+  <si>
+    <t>Develop and implement training programs for customer support staff</t>
+  </si>
+  <si>
+    <t>Coordinate with the marketing team for promotional campaigns</t>
+  </si>
+  <si>
+    <t>Prepare and present business cases for new investment opportunities</t>
+  </si>
+  <si>
+    <t>Monitor and optimize website SEO performance</t>
+  </si>
+  <si>
+    <t>Coordinate with the procurement team for vendor selection</t>
+  </si>
+  <si>
+    <t>Review and approve marketing collateral designs</t>
+  </si>
+  <si>
+    <t>Prepare and conduct employee onboarding sessions</t>
+  </si>
+  <si>
+    <t>Coordinate with the manufacturing team for production planning</t>
+  </si>
+  <si>
+    <t>Analyze market trends and make pricing recommendations</t>
+  </si>
+  <si>
+    <t>Respond to customer inquiries via live chat support</t>
+  </si>
+  <si>
+    <t>Conduct user testing sessions for software usability assessment</t>
+  </si>
+  <si>
+    <t>Develop and implement performance improvement plans for underperforming employees</t>
   </si>
 </sst>
 </file>
@@ -568,15 +862,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="D239" sqref="D239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" customWidth="1"/>
+    <col min="1" max="1" width="78.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1140,6 +1434,1350 @@
         <v>5</v>
       </c>
     </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>82</v>
+      </c>
+      <c r="B91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>83</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>87</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>88</v>
+      </c>
+      <c r="B97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>89</v>
+      </c>
+      <c r="B98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>90</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>92</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>96</v>
+      </c>
+      <c r="B105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>97</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>98</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>99</v>
+      </c>
+      <c r="B108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>100</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>101</v>
+      </c>
+      <c r="B110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>102</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>19</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>20</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>21</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>22</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>24</v>
+      </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>25</v>
+      </c>
+      <c r="B119">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>103</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>104</v>
+      </c>
+      <c r="B121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>105</v>
+      </c>
+      <c r="B122">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>106</v>
+      </c>
+      <c r="B123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>107</v>
+      </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>108</v>
+      </c>
+      <c r="B125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>109</v>
+      </c>
+      <c r="B126">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>110</v>
+      </c>
+      <c r="B127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>111</v>
+      </c>
+      <c r="B128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>112</v>
+      </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>113</v>
+      </c>
+      <c r="B130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>114</v>
+      </c>
+      <c r="B131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>115</v>
+      </c>
+      <c r="B132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>116</v>
+      </c>
+      <c r="B133">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>117</v>
+      </c>
+      <c r="B134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>118</v>
+      </c>
+      <c r="B135">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>119</v>
+      </c>
+      <c r="B136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>120</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>121</v>
+      </c>
+      <c r="B138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>122</v>
+      </c>
+      <c r="B139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>18</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>19</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>20</v>
+      </c>
+      <c r="B142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>21</v>
+      </c>
+      <c r="B143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>22</v>
+      </c>
+      <c r="B144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>23</v>
+      </c>
+      <c r="B145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>24</v>
+      </c>
+      <c r="B146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>25</v>
+      </c>
+      <c r="B147">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>78</v>
+      </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>79</v>
+      </c>
+      <c r="B149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>80</v>
+      </c>
+      <c r="B150">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>81</v>
+      </c>
+      <c r="B151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>82</v>
+      </c>
+      <c r="B152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>83</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>84</v>
+      </c>
+      <c r="B154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>85</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>86</v>
+      </c>
+      <c r="B156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>87</v>
+      </c>
+      <c r="B157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>88</v>
+      </c>
+      <c r="B158">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>89</v>
+      </c>
+      <c r="B159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>90</v>
+      </c>
+      <c r="B160">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>91</v>
+      </c>
+      <c r="B161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>92</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>93</v>
+      </c>
+      <c r="B163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>94</v>
+      </c>
+      <c r="B164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>95</v>
+      </c>
+      <c r="B165">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>96</v>
+      </c>
+      <c r="B166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>97</v>
+      </c>
+      <c r="B167">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>98</v>
+      </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>99</v>
+      </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>100</v>
+      </c>
+      <c r="B170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>101</v>
+      </c>
+      <c r="B171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>102</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>103</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>104</v>
+      </c>
+      <c r="B174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>105</v>
+      </c>
+      <c r="B175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>106</v>
+      </c>
+      <c r="B176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>107</v>
+      </c>
+      <c r="B177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>108</v>
+      </c>
+      <c r="B178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>109</v>
+      </c>
+      <c r="B179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>110</v>
+      </c>
+      <c r="B180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>111</v>
+      </c>
+      <c r="B181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>112</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>113</v>
+      </c>
+      <c r="B183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>114</v>
+      </c>
+      <c r="B184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>115</v>
+      </c>
+      <c r="B185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>116</v>
+      </c>
+      <c r="B186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>117</v>
+      </c>
+      <c r="B187">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>118</v>
+      </c>
+      <c r="B188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>119</v>
+      </c>
+      <c r="B189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>120</v>
+      </c>
+      <c r="B190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>121</v>
+      </c>
+      <c r="B191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>122</v>
+      </c>
+      <c r="B192">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>123</v>
+      </c>
+      <c r="B193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>124</v>
+      </c>
+      <c r="B194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>125</v>
+      </c>
+      <c r="B195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>126</v>
+      </c>
+      <c r="B196">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>127</v>
+      </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>128</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>129</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>130</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>131</v>
+      </c>
+      <c r="B201">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>132</v>
+      </c>
+      <c r="B202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>133</v>
+      </c>
+      <c r="B203">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>134</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>135</v>
+      </c>
+      <c r="B205">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>136</v>
+      </c>
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>137</v>
+      </c>
+      <c r="B207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>138</v>
+      </c>
+      <c r="B208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>139</v>
+      </c>
+      <c r="B209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>140</v>
+      </c>
+      <c r="B210">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>141</v>
+      </c>
+      <c r="B211">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>142</v>
+      </c>
+      <c r="B212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>143</v>
+      </c>
+      <c r="B213">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>144</v>
+      </c>
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>145</v>
+      </c>
+      <c r="B215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>146</v>
+      </c>
+      <c r="B216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>147</v>
+      </c>
+      <c r="B217">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>148</v>
+      </c>
+      <c r="B218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>149</v>
+      </c>
+      <c r="B219">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>150</v>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>151</v>
+      </c>
+      <c r="B221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>152</v>
+      </c>
+      <c r="B222">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>153</v>
+      </c>
+      <c r="B223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>154</v>
+      </c>
+      <c r="B224">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>155</v>
+      </c>
+      <c r="B225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>156</v>
+      </c>
+      <c r="B226">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>157</v>
+      </c>
+      <c r="B227">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>158</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>159</v>
+      </c>
+      <c r="B229">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>160</v>
+      </c>
+      <c r="B230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>161</v>
+      </c>
+      <c r="B231">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>162</v>
+      </c>
+      <c r="B232">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>163</v>
+      </c>
+      <c r="B233">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>164</v>
+      </c>
+      <c r="B234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>165</v>
+      </c>
+      <c r="B235">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>166</v>
+      </c>
+      <c r="B236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>167</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>168</v>
+      </c>
+      <c r="B238">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>